<commit_message>
better spidercharts and clustering added
</commit_message>
<xml_diff>
--- a/data/raw/riparu_typologie_sites.xlsx
+++ b/data/raw/riparu_typologie_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\work\stareso\etudes\marevivu\riparu\riparuR\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F3F8C7-1365-45FB-9A45-DCB3923F81E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA2788-BF69-42D1-A68D-51937C829FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -1661,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249339E7-85A2-4BBD-B4D8-66D39A505D8C}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2342,8 +2342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
metadata completion previously not saved
</commit_message>
<xml_diff>
--- a/data/raw/riparu_typologie_sites.xlsx
+++ b/data/raw/riparu_typologie_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\work\stareso\etudes\marevivu\riparu\riparuR\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA2788-BF69-42D1-A68D-51937C829FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1080D0-8C29-42BB-A639-F92B4144CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="232">
   <si>
     <t xml:space="preserve">MV </t>
   </si>
@@ -528,9 +528,6 @@
     <t>facteur</t>
   </si>
   <si>
-    <t>reels</t>
-  </si>
-  <si>
     <t>Type d'arrière plage</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
     <t>liste de réels</t>
   </si>
   <si>
-    <t>réel</t>
-  </si>
-  <si>
     <t>km</t>
   </si>
   <si>
@@ -739,6 +733,12 @@
   </si>
   <si>
     <t>Nom du site de la plage étudiée où est effectué le transect</t>
+  </si>
+  <si>
+    <t>reel</t>
+  </si>
+  <si>
+    <t>liste de reels</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249339E7-85A2-4BBD-B4D8-66D39A505D8C}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C2" s="38" t="s">
         <v>139</v>
@@ -1711,7 +1711,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>139</v>
@@ -1729,7 +1729,7 @@
         <v>158</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>138</v>
@@ -1774,7 +1774,7 @@
         <v>149</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>201</v>
+        <v>231</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>138</v>
@@ -1789,7 +1789,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>201</v>
+        <v>231</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>138</v>
@@ -1807,7 +1807,7 @@
         <v>160</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -1822,7 +1822,7 @@
         <v>160</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E10" s="29"/>
     </row>
@@ -1837,7 +1837,7 @@
         <v>160</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -1849,10 +1849,10 @@
         <v>154</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>161</v>
+        <v>230</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" s="29"/>
     </row>
@@ -1867,7 +1867,7 @@
         <v>160</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="29"/>
     </row>
@@ -1882,7 +1882,7 @@
         <v>160</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E14" s="29"/>
     </row>
@@ -1891,13 +1891,13 @@
         <v>83</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E15" s="28"/>
     </row>
@@ -1915,7 +1915,7 @@
         <v>158</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
@@ -1923,60 +1923,60 @@
         <v>85</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D17" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>163</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1">
       <c r="A18" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1">
       <c r="A19" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E19" s="40"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E20" s="30"/>
     </row>
@@ -1997,16 +1997,16 @@
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1">
       <c r="A22" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E22" s="30"/>
     </row>
@@ -2015,88 +2015,88 @@
         <v>88</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1">
       <c r="A24" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E24" s="30"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1">
       <c r="A25" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" s="30"/>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1">
       <c r="A26" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="50" t="s">
         <v>193</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>194</v>
       </c>
       <c r="C26" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E26" s="30"/>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1">
       <c r="A27" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="30"/>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1">
       <c r="A28" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" s="40" t="s">
         <v>160</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E28" s="30"/>
     </row>
@@ -2105,7 +2105,7 @@
         <v>89</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" s="54" t="s">
         <v>139</v>
@@ -2120,13 +2120,13 @@
         <v>90</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E30" s="31"/>
     </row>
@@ -2135,13 +2135,13 @@
         <v>91</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>160</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E31" s="31"/>
     </row>
@@ -2150,10 +2150,14 @@
         <v>105</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>205</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+        <v>203</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" ht="30" customHeight="1">
@@ -2161,10 +2165,14 @@
         <v>106</v>
       </c>
       <c r="B33" s="53" t="s">
-        <v>206</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+        <v>204</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>201</v>
+      </c>
       <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1">
@@ -2172,13 +2180,13 @@
         <v>108</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>160</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E34" s="31"/>
     </row>
@@ -2187,10 +2195,14 @@
         <v>107</v>
       </c>
       <c r="B35" s="54" t="s">
-        <v>208</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+        <v>206</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="E35" s="31"/>
     </row>
     <row r="36" spans="1:5" ht="30" customHeight="1">
@@ -2198,10 +2210,14 @@
         <v>118</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+        <v>208</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1">
@@ -2209,10 +2225,14 @@
         <v>116</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+        <v>209</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>201</v>
+      </c>
       <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5" ht="30" customHeight="1">
@@ -2220,13 +2240,13 @@
         <v>117</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C38" s="31" t="s">
         <v>160</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E38" s="31"/>
     </row>
@@ -2235,10 +2255,14 @@
         <v>119</v>
       </c>
       <c r="B39" s="53" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+        <v>211</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>100</v>
+      </c>
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" ht="30" customHeight="1">
@@ -2246,10 +2270,14 @@
         <v>120</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>214</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+        <v>212</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>201</v>
+      </c>
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" ht="33.75" customHeight="1">
@@ -2257,13 +2285,13 @@
         <v>121</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C41" s="31" t="s">
         <v>160</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E41" s="31"/>
     </row>
@@ -2272,12 +2300,14 @@
         <v>125</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C42" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="32"/>
+      <c r="D42" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" ht="30" customHeight="1">
@@ -2285,12 +2315,14 @@
         <v>126</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C43" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="32"/>
+      <c r="D43" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="E43" s="32"/>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1">
@@ -2298,12 +2330,14 @@
         <v>127</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C44" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="32"/>
+      <c r="D44" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="E44" s="32"/>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1">
@@ -2316,7 +2350,9 @@
       <c r="C45" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D45" s="34"/>
+      <c r="D45" s="34" t="s">
+        <v>100</v>
+      </c>
       <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1">
@@ -2329,7 +2365,9 @@
       <c r="C46" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="36"/>
+      <c r="D46" s="34" t="s">
+        <v>100</v>
+      </c>
       <c r="E46" s="36"/>
     </row>
   </sheetData>
@@ -2342,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2387,7 +2425,7 @@
   <sheetData>
     <row r="1" spans="1:51" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>75</v>
@@ -2435,37 +2473,37 @@
         <v>85</v>
       </c>
       <c r="Q1" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>167</v>
       </c>
       <c r="T1" s="18" t="s">
         <v>87</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="V1" s="18" t="s">
         <v>88</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Z1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA1" s="18" t="s">
         <v>190</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>191</v>
       </c>
       <c r="AB1" s="19" t="s">
         <v>89</v>
@@ -2563,7 +2601,7 @@
         <v>70</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O2" s="44" t="s">
         <v>100</v>
@@ -2584,7 +2622,7 @@
         <v>100</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V2" s="39" t="s">
         <v>71</v>
@@ -2596,7 +2634,7 @@
         <v>70</v>
       </c>
       <c r="Y2" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>7</v>
@@ -2700,7 +2738,7 @@
         <v>70</v>
       </c>
       <c r="N3" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>100</v>
@@ -2721,7 +2759,7 @@
         <v>100</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V3" s="39" t="s">
         <v>71</v>
@@ -2733,7 +2771,7 @@
         <v>70</v>
       </c>
       <c r="Y3" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>18</v>
@@ -2781,7 +2819,7 @@
         <v>124</v>
       </c>
       <c r="AO3" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP3" s="39" t="s">
         <v>100</v>
@@ -2837,7 +2875,7 @@
         <v>70</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O4" s="44" t="s">
         <v>100</v>
@@ -2858,7 +2896,7 @@
         <v>100</v>
       </c>
       <c r="U4" s="39" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="V4" s="39" t="s">
         <v>71</v>
@@ -2870,7 +2908,7 @@
         <v>70</v>
       </c>
       <c r="Y4" s="39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>26</v>
@@ -2974,7 +3012,7 @@
         <v>70</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O5" s="44" t="s">
         <v>100</v>
@@ -2995,7 +3033,7 @@
         <v>100</v>
       </c>
       <c r="U5" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V5" s="39" t="s">
         <v>71</v>
@@ -3007,13 +3045,13 @@
         <v>71</v>
       </c>
       <c r="Y5" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z5" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA5" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>94</v>
@@ -3055,7 +3093,7 @@
         <v>58</v>
       </c>
       <c r="AO5" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP5" s="45" t="s">
         <v>100</v>
@@ -3067,7 +3105,7 @@
         <v>134</v>
       </c>
       <c r="AS5" s="57" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="24" customHeight="1">
@@ -3111,7 +3149,7 @@
         <v>70</v>
       </c>
       <c r="N6" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O6" s="44" t="s">
         <v>100</v>
@@ -3132,7 +3170,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V6" s="39" t="s">
         <v>71</v>
@@ -3144,7 +3182,7 @@
         <v>70</v>
       </c>
       <c r="Y6" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>7</v>
@@ -3192,7 +3230,7 @@
         <v>58</v>
       </c>
       <c r="AO6" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP6" s="39" t="s">
         <v>100</v>
@@ -3248,7 +3286,7 @@
         <v>70</v>
       </c>
       <c r="N7" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>100</v>
@@ -3269,7 +3307,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="39" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="V7" s="39" t="s">
         <v>71</v>
@@ -3281,7 +3319,7 @@
         <v>70</v>
       </c>
       <c r="Y7" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>44</v>
@@ -3329,7 +3367,7 @@
         <v>65</v>
       </c>
       <c r="AO7" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP7" s="39" t="s">
         <v>100</v>
@@ -3385,7 +3423,7 @@
         <v>70</v>
       </c>
       <c r="N8" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>100</v>
@@ -3406,7 +3444,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V8" s="39" t="s">
         <v>71</v>
@@ -3418,13 +3456,13 @@
         <v>71</v>
       </c>
       <c r="Y8" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z8" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA8" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>97</v>
@@ -3466,7 +3504,7 @@
         <v>124</v>
       </c>
       <c r="AO8" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP8" s="39" t="s">
         <v>100</v>
@@ -3522,7 +3560,7 @@
         <v>70</v>
       </c>
       <c r="N9" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O9" s="44" t="s">
         <v>100</v>
@@ -3543,10 +3581,10 @@
         <v>100</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V9" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="W9" s="5" t="s">
         <v>7</v>
@@ -3555,7 +3593,7 @@
         <v>70</v>
       </c>
       <c r="Y9" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>6</v>
@@ -3603,7 +3641,7 @@
         <v>18</v>
       </c>
       <c r="AO9" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP9" s="39" t="s">
         <v>100</v>
@@ -3659,7 +3697,7 @@
         <v>70</v>
       </c>
       <c r="N10" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O10" s="44" t="s">
         <v>100</v>
@@ -3680,7 +3718,7 @@
         <v>100</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="V10" s="39" t="s">
         <v>71</v>
@@ -3692,13 +3730,13 @@
         <v>71</v>
       </c>
       <c r="Y10" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z10" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA10" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>98</v>
@@ -3740,7 +3778,7 @@
         <v>18</v>
       </c>
       <c r="AO10" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AP10" s="39" t="s">
         <v>100</v>
@@ -3796,7 +3834,7 @@
         <v>70</v>
       </c>
       <c r="N11" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O11" s="44" t="s">
         <v>100</v>
@@ -3817,7 +3855,7 @@
         <v>100</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="V11" s="39" t="s">
         <v>71</v>
@@ -3829,7 +3867,7 @@
         <v>70</v>
       </c>
       <c r="Y11" s="39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>7</v>
@@ -3880,7 +3918,7 @@
         <v>131</v>
       </c>
       <c r="AP11" s="39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AQ11" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
no use of macrodechets_essentiel so deleted
</commit_message>
<xml_diff>
--- a/data/raw/riparu_typologie_sites.xlsx
+++ b/data/raw/riparu_typologie_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\work\stareso\etudes\marevivu\riparu\riparuR\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1080D0-8C29-42BB-A639-F92B4144CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3460A2CA-1318-4A24-8678-79E4BF8D54B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="3915" windowWidth="28800" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -1661,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249339E7-85A2-4BBD-B4D8-66D39A505D8C}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -2380,8 +2380,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2646,7 +2649,7 @@
         <v>92</v>
       </c>
       <c r="AC2" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>65</v>
@@ -2783,7 +2786,7 @@
         <v>92</v>
       </c>
       <c r="AC3" s="5">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>18</v>
@@ -3468,7 +3471,7 @@
         <v>97</v>
       </c>
       <c r="AC8" s="5">
-        <v>18.8</v>
+        <v>0.2</v>
       </c>
       <c r="AD8" s="5" t="s">
         <v>65</v>
@@ -3605,7 +3608,7 @@
         <v>97</v>
       </c>
       <c r="AC9" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="AD9" s="5" t="s">
         <v>65</v>
@@ -3879,7 +3882,7 @@
         <v>99</v>
       </c>
       <c r="AC11" s="5">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AD11" s="5" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
changes with surface value computation and not 100m assuming that all transects are 100m (could change in the future)
</commit_message>
<xml_diff>
--- a/data/raw/riparu_typologie_sites.xlsx
+++ b/data/raw/riparu_typologie_sites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\work\stareso\etudes\marevivu\riparu\riparuR\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3460A2CA-1318-4A24-8678-79E4BF8D54B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86246E9-5690-4F9E-880E-80B6DA78C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="3915" windowWidth="28800" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="4" r:id="rId1"/>
@@ -453,12 +453,6 @@
     <t xml:space="preserve">PNMCCA  </t>
   </si>
   <si>
-    <t>transect_longueur</t>
-  </si>
-  <si>
-    <t>transect_largeur</t>
-  </si>
-  <si>
     <t>degrés decimaux</t>
   </si>
   <si>
@@ -483,9 +477,6 @@
     <t>Aucune</t>
   </si>
   <si>
-    <t>Longueur du transect</t>
-  </si>
-  <si>
     <t>Largeur du transect</t>
   </si>
   <si>
@@ -739,6 +730,15 @@
   </si>
   <si>
     <t>liste de reels</t>
+  </si>
+  <si>
+    <t>plage_longueur</t>
+  </si>
+  <si>
+    <t>plage_largeur</t>
+  </si>
+  <si>
+    <t>Longueur de la plage</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249339E7-85A2-4BBD-B4D8-66D39A505D8C}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1676,30 +1676,30 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
       <c r="A1" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>142</v>
-      </c>
       <c r="C1" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>100</v>
@@ -1711,10 +1711,10 @@
         <v>75</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>100</v>
@@ -1726,25 +1726,25 @@
         <v>76</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>136</v>
+        <v>229</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>146</v>
+        <v>231</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>133</v>
@@ -1753,13 +1753,13 @@
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>133</v>
@@ -1771,13 +1771,13 @@
         <v>77</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -1786,13 +1786,13 @@
         <v>78</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -1801,13 +1801,13 @@
         <v>79</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -1816,13 +1816,13 @@
         <v>80</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E10" s="29"/>
     </row>
@@ -1831,13 +1831,13 @@
         <v>81</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -1846,13 +1846,13 @@
         <v>82</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E12" s="29"/>
     </row>
@@ -1861,13 +1861,13 @@
         <v>69</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E13" s="29"/>
     </row>
@@ -1876,13 +1876,13 @@
         <v>72</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E14" s="29"/>
     </row>
@@ -1891,13 +1891,13 @@
         <v>83</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E15" s="28"/>
     </row>
@@ -1906,16 +1906,16 @@
         <v>84</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1">
@@ -1923,60 +1923,60 @@
         <v>85</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C17" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>160</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1">
       <c r="A18" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="C18" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>167</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>170</v>
       </c>
       <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1">
       <c r="A19" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="50" t="s">
-        <v>168</v>
-      </c>
       <c r="C19" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E19" s="40"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1">
       <c r="A20" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="50" t="s">
-        <v>169</v>
-      </c>
       <c r="C20" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E20" s="30"/>
     </row>
@@ -1985,28 +1985,28 @@
         <v>87</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1">
       <c r="A22" s="41" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B22" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="40" t="s">
         <v>174</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>177</v>
       </c>
       <c r="E22" s="30"/>
     </row>
@@ -2015,88 +2015,88 @@
         <v>88</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1">
       <c r="A24" s="41" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E24" s="30"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1">
       <c r="A25" s="41" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E25" s="30"/>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1">
       <c r="A26" s="41" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E26" s="30"/>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1">
       <c r="A27" s="41" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E27" s="30"/>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1">
       <c r="A28" s="41" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E28" s="30"/>
     </row>
@@ -2105,10 +2105,10 @@
         <v>89</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D29" s="54" t="s">
         <v>100</v>
@@ -2120,13 +2120,13 @@
         <v>90</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D30" s="54" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E30" s="31"/>
     </row>
@@ -2135,13 +2135,13 @@
         <v>91</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E31" s="31"/>
     </row>
@@ -2150,10 +2150,10 @@
         <v>105</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D32" s="31" t="s">
         <v>100</v>
@@ -2165,13 +2165,13 @@
         <v>106</v>
       </c>
       <c r="B33" s="53" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E33" s="31"/>
     </row>
@@ -2180,13 +2180,13 @@
         <v>108</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E34" s="31"/>
     </row>
@@ -2195,10 +2195,10 @@
         <v>107</v>
       </c>
       <c r="B35" s="54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>100</v>
@@ -2210,10 +2210,10 @@
         <v>118</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D36" s="31" t="s">
         <v>100</v>
@@ -2225,13 +2225,13 @@
         <v>116</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E37" s="31"/>
     </row>
@@ -2240,13 +2240,13 @@
         <v>117</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E38" s="31"/>
     </row>
@@ -2255,10 +2255,10 @@
         <v>119</v>
       </c>
       <c r="B39" s="53" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>100</v>
@@ -2270,13 +2270,13 @@
         <v>120</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E40" s="31"/>
     </row>
@@ -2285,13 +2285,13 @@
         <v>121</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E41" s="31"/>
     </row>
@@ -2300,10 +2300,10 @@
         <v>125</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C42" s="56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D42" s="32" t="s">
         <v>100</v>
@@ -2315,10 +2315,10 @@
         <v>126</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D43" s="32" t="s">
         <v>100</v>
@@ -2330,10 +2330,10 @@
         <v>127</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D44" s="32" t="s">
         <v>100</v>
@@ -2345,10 +2345,10 @@
         <v>73</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>100</v>
@@ -2360,10 +2360,10 @@
         <v>74</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D46" s="34" t="s">
         <v>100</v>
@@ -2380,11 +2380,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE22" sqref="AE22"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2428,7 +2428,7 @@
   <sheetData>
     <row r="1" spans="1:51" s="6" customFormat="1" ht="38.25" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>75</v>
@@ -2437,10 +2437,10 @@
         <v>76</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>136</v>
+        <v>229</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>77</v>
@@ -2476,37 +2476,37 @@
         <v>85</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T1" s="18" t="s">
         <v>87</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="V1" s="18" t="s">
         <v>88</v>
       </c>
       <c r="W1" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="X1" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="X1" s="18" t="s">
-        <v>179</v>
-      </c>
       <c r="Y1" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AB1" s="19" t="s">
         <v>89</v>
@@ -2604,7 +2604,7 @@
         <v>70</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O2" s="44" t="s">
         <v>100</v>
@@ -2625,7 +2625,7 @@
         <v>100</v>
       </c>
       <c r="U2" s="39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V2" s="39" t="s">
         <v>71</v>
@@ -2637,7 +2637,7 @@
         <v>70</v>
       </c>
       <c r="Y2" s="39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>7</v>
@@ -2741,7 +2741,7 @@
         <v>70</v>
       </c>
       <c r="N3" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O3" s="44" t="s">
         <v>100</v>
@@ -2762,7 +2762,7 @@
         <v>100</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V3" s="39" t="s">
         <v>71</v>
@@ -2774,7 +2774,7 @@
         <v>70</v>
       </c>
       <c r="Y3" s="39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>18</v>
@@ -2822,7 +2822,7 @@
         <v>124</v>
       </c>
       <c r="AO3" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP3" s="39" t="s">
         <v>100</v>
@@ -2878,7 +2878,7 @@
         <v>70</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O4" s="44" t="s">
         <v>100</v>
@@ -2899,7 +2899,7 @@
         <v>100</v>
       </c>
       <c r="U4" s="39" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="V4" s="39" t="s">
         <v>71</v>
@@ -2911,7 +2911,7 @@
         <v>70</v>
       </c>
       <c r="Y4" s="39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>26</v>
@@ -2971,7 +2971,7 @@
         <v>19</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:51" ht="24" customHeight="1">
@@ -3015,7 +3015,7 @@
         <v>70</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O5" s="44" t="s">
         <v>100</v>
@@ -3036,7 +3036,7 @@
         <v>100</v>
       </c>
       <c r="U5" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="V5" s="39" t="s">
         <v>71</v>
@@ -3048,13 +3048,13 @@
         <v>71</v>
       </c>
       <c r="Y5" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Z5" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA5" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>94</v>
@@ -3096,7 +3096,7 @@
         <v>58</v>
       </c>
       <c r="AO5" s="45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP5" s="45" t="s">
         <v>100</v>
@@ -3108,7 +3108,7 @@
         <v>134</v>
       </c>
       <c r="AS5" s="57" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:51" ht="24" customHeight="1">
@@ -3152,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="N6" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O6" s="44" t="s">
         <v>100</v>
@@ -3173,7 +3173,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V6" s="39" t="s">
         <v>71</v>
@@ -3185,7 +3185,7 @@
         <v>70</v>
       </c>
       <c r="Y6" s="39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>7</v>
@@ -3233,7 +3233,7 @@
         <v>58</v>
       </c>
       <c r="AO6" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP6" s="39" t="s">
         <v>100</v>
@@ -3289,7 +3289,7 @@
         <v>70</v>
       </c>
       <c r="N7" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O7" s="44" t="s">
         <v>100</v>
@@ -3310,7 +3310,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="39" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="V7" s="39" t="s">
         <v>71</v>
@@ -3322,7 +3322,7 @@
         <v>70</v>
       </c>
       <c r="Y7" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>44</v>
@@ -3370,7 +3370,7 @@
         <v>65</v>
       </c>
       <c r="AO7" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP7" s="39" t="s">
         <v>100</v>
@@ -3382,7 +3382,7 @@
         <v>11</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:51" ht="24" customHeight="1">
@@ -3426,7 +3426,7 @@
         <v>70</v>
       </c>
       <c r="N8" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O8" s="44" t="s">
         <v>100</v>
@@ -3447,7 +3447,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="V8" s="39" t="s">
         <v>71</v>
@@ -3459,13 +3459,13 @@
         <v>71</v>
       </c>
       <c r="Y8" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Z8" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA8" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>97</v>
@@ -3507,7 +3507,7 @@
         <v>124</v>
       </c>
       <c r="AO8" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP8" s="39" t="s">
         <v>100</v>
@@ -3563,7 +3563,7 @@
         <v>70</v>
       </c>
       <c r="N9" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O9" s="44" t="s">
         <v>100</v>
@@ -3584,10 +3584,10 @@
         <v>100</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="V9" s="39" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="W9" s="5" t="s">
         <v>7</v>
@@ -3596,7 +3596,7 @@
         <v>70</v>
       </c>
       <c r="Y9" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>6</v>
@@ -3644,7 +3644,7 @@
         <v>18</v>
       </c>
       <c r="AO9" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP9" s="39" t="s">
         <v>100</v>
@@ -3656,7 +3656,7 @@
         <v>11</v>
       </c>
       <c r="AS9" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:51" ht="24" customHeight="1">
@@ -3700,7 +3700,7 @@
         <v>70</v>
       </c>
       <c r="N10" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O10" s="44" t="s">
         <v>100</v>
@@ -3721,7 +3721,7 @@
         <v>100</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="V10" s="39" t="s">
         <v>71</v>
@@ -3733,13 +3733,13 @@
         <v>71</v>
       </c>
       <c r="Y10" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Z10" s="39" t="s">
         <v>100</v>
       </c>
       <c r="AA10" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>98</v>
@@ -3781,7 +3781,7 @@
         <v>18</v>
       </c>
       <c r="AO10" s="39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AP10" s="39" t="s">
         <v>100</v>
@@ -3837,7 +3837,7 @@
         <v>70</v>
       </c>
       <c r="N11" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O11" s="44" t="s">
         <v>100</v>
@@ -3858,7 +3858,7 @@
         <v>100</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="V11" s="39" t="s">
         <v>71</v>
@@ -3870,7 +3870,7 @@
         <v>70</v>
       </c>
       <c r="Y11" s="39" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>7</v>
@@ -3921,7 +3921,7 @@
         <v>131</v>
       </c>
       <c r="AP11" s="39" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AQ11" s="5" t="s">
         <v>10</v>

</xml_diff>